<commit_message>
Add voting rollup, clean up XLSX data, closes #13
</commit_message>
<xml_diff>
--- a/data/cleaned/voting/TX-scorecard-2013.xlsx
+++ b/data/cleaned/voting/TX-scorecard-2013.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dan/working/enviro_papers/data/cleaned/voting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65CA120-3638-3F46-ADB6-689C8820E1CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0672294C-6A20-3847-9A2B-9ABFA22C3554}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="19920" windowHeight="13000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3754,6 +3754,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <cols>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="5" t="s">

</xml_diff>